<commit_message>
Done with copy scripts
</commit_message>
<xml_diff>
--- a/Seasons/data/beach_seasons_all_2020.xlsx
+++ b/Seasons/data/beach_seasons_all_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\RStudio\intertidal\Seasons\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA8C5DE-4F35-441B-B2DC-C6F74EE9CC48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AAE29A-D625-434B-A458-9ECA60938C00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13695" yWindow="7560" windowWidth="25260" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="39" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>b8698acb-f324-474a-9bc3-4d16bd7ffbc7</t>
   </si>
   <si>
-    <t>3ba0ab83-643e-4808-8555-eed517678f2</t>
-  </si>
-  <si>
     <t>9361bb23-67e1-4698-a603-3a463ac028c2</t>
   </si>
   <si>
@@ -300,9 +297,6 @@
     <t>Pt Whitney Tidelands</t>
   </si>
   <si>
-    <t>0f05f34f-d3ae-4904-b6db-a08875f190d</t>
-  </si>
-  <si>
     <t>c08e7d0c-7c27-4b3c-a0bb-d83709ead77d</t>
   </si>
   <si>
@@ -358,6 +352,12 @@
   </si>
   <si>
     <t>Wolfe Prop. SP</t>
+  </si>
+  <si>
+    <t>3ba0ab83-643e-4808-8555-eed517678f24</t>
+  </si>
+  <si>
+    <t>0f05f34f-d3ae-4904-b6db-a08875f190d1</t>
   </si>
 </sst>
 </file>
@@ -1218,13 +1218,13 @@
   <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="A122:A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
@@ -2422,13 +2422,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="2">
         <v>250014</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
@@ -2454,13 +2454,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="2">
         <v>250014</v>
       </c>
       <c r="C39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
@@ -2486,13 +2486,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B40" s="2">
         <v>250014</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -2518,13 +2518,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41" s="2">
         <v>250014</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -2550,13 +2550,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" s="2">
         <v>250014</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B43" s="2">
         <v>250014</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
         <v>17</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B44" s="2">
         <v>270300</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B45" s="2">
         <v>270300</v>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B46" s="2">
         <v>270300</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B47" s="2">
         <v>270300</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B48" s="2">
         <v>270300</v>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B49" s="2">
         <v>270300</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B50" s="2">
         <v>270300</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B51" s="2">
         <v>270300</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" s="2">
         <v>250260</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" s="2">
         <v>250260</v>
@@ -2934,7 +2934,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" s="2">
         <v>250260</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" s="2">
         <v>250260</v>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="2">
         <v>250260</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="2">
         <v>250260</v>
@@ -3062,7 +3062,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="2">
         <v>240440</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="2">
         <v>240440</v>
@@ -3126,7 +3126,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" s="2">
         <v>240440</v>
@@ -3158,7 +3158,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61" s="2">
         <v>240440</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62" s="2">
         <v>240440</v>
@@ -3222,7 +3222,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B63" s="2">
         <v>240440</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64" s="2">
         <v>281140</v>
       </c>
       <c r="C64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
@@ -3286,13 +3286,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B65" s="2">
         <v>281140</v>
       </c>
       <c r="C65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>
@@ -3318,13 +3318,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" s="2">
         <v>281140</v>
       </c>
       <c r="C66" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
@@ -3350,13 +3350,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" s="2">
         <v>281140</v>
       </c>
       <c r="C67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
@@ -3382,13 +3382,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" s="2">
         <v>281140</v>
       </c>
       <c r="C68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D68" t="s">
         <v>17</v>
@@ -3414,13 +3414,13 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69" s="2">
         <v>281140</v>
       </c>
       <c r="C69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D69" t="s">
         <v>17</v>
@@ -3446,13 +3446,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B70" s="2">
         <v>280975</v>
       </c>
       <c r="C70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D70" t="s">
         <v>17</v>
@@ -3478,13 +3478,13 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B71" s="2">
         <v>280975</v>
       </c>
       <c r="C71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D71" t="s">
         <v>17</v>
@@ -3510,13 +3510,13 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B72" s="2">
         <v>280975</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -3542,13 +3542,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B73" s="2">
         <v>280975</v>
       </c>
       <c r="C73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
@@ -3574,13 +3574,13 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" s="2">
         <v>280975</v>
       </c>
       <c r="C74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D74" t="s">
         <v>17</v>
@@ -3606,13 +3606,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B75" s="2">
         <v>280975</v>
       </c>
       <c r="C75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D75" t="s">
         <v>17</v>
@@ -3638,13 +3638,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B76" s="2">
         <v>260380</v>
       </c>
       <c r="C76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D76" t="s">
         <v>17</v>
@@ -3670,13 +3670,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B77" s="2">
         <v>260380</v>
       </c>
       <c r="C77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D77" t="s">
         <v>17</v>
@@ -3702,13 +3702,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" s="2">
         <v>260380</v>
       </c>
       <c r="C78" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
@@ -3734,13 +3734,13 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B79" s="2">
         <v>260380</v>
       </c>
       <c r="C79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D79" t="s">
         <v>12</v>
@@ -3766,13 +3766,13 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B80" s="2">
         <v>260380</v>
       </c>
       <c r="C80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D80" t="s">
         <v>17</v>
@@ -3798,13 +3798,13 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B81" s="2">
         <v>260380</v>
       </c>
       <c r="C81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D81" t="s">
         <v>17</v>
@@ -3830,7 +3830,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B82" s="2">
         <v>250410</v>
@@ -3862,7 +3862,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B83" s="2">
         <v>250410</v>
@@ -3894,7 +3894,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B84" s="2">
         <v>250410</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B85" s="2">
         <v>250410</v>
@@ -3958,7 +3958,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B86" s="2">
         <v>250410</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B87" s="2">
         <v>250410</v>
@@ -4022,7 +4022,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B88" s="2">
         <v>270230</v>
@@ -4054,7 +4054,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B89" s="2">
         <v>270230</v>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B90" s="2">
         <v>280570</v>
@@ -4118,7 +4118,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B91" s="2">
         <v>280570</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B92" s="2">
         <v>250300</v>
@@ -4182,7 +4182,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B93" s="2">
         <v>250300</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B94" s="2">
         <v>250300</v>
@@ -4246,7 +4246,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B95" s="2">
         <v>250300</v>
@@ -4278,7 +4278,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B96" s="2">
         <v>250300</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B97" s="2">
         <v>250300</v>
@@ -4342,13 +4342,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B98" s="2">
         <v>280711</v>
       </c>
       <c r="C98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D98" t="s">
         <v>17</v>
@@ -4374,13 +4374,13 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B99" s="2">
         <v>280711</v>
       </c>
       <c r="C99" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D99" t="s">
         <v>17</v>
@@ -4406,13 +4406,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B100" s="2">
         <v>280711</v>
       </c>
       <c r="C100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D100" t="s">
         <v>12</v>
@@ -4438,13 +4438,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B101" s="2">
         <v>280711</v>
       </c>
       <c r="C101" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D101" t="s">
         <v>12</v>
@@ -4470,13 +4470,13 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B102" s="2">
         <v>280711</v>
       </c>
       <c r="C102" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D102" t="s">
         <v>17</v>
@@ -4502,13 +4502,13 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B103" s="2">
         <v>280711</v>
       </c>
       <c r="C103" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D103" t="s">
         <v>17</v>
@@ -4534,13 +4534,13 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B104" s="2">
         <v>280711</v>
       </c>
       <c r="C104" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D104" t="s">
         <v>12</v>
@@ -4566,13 +4566,13 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B105" s="2">
         <v>280711</v>
       </c>
       <c r="C105" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D105" t="s">
         <v>12</v>
@@ -4598,13 +4598,13 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B106" s="2">
         <v>280711</v>
       </c>
       <c r="C106" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D106" t="s">
         <v>17</v>
@@ -4630,13 +4630,13 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B107" s="2">
         <v>280711</v>
       </c>
       <c r="C107" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D107" t="s">
         <v>17</v>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B108" s="2">
         <v>250400</v>
@@ -4694,7 +4694,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B109" s="2">
         <v>250400</v>
@@ -4726,7 +4726,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B110" s="2">
         <v>280680</v>
@@ -4758,7 +4758,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B111" s="2">
         <v>280680</v>
@@ -4790,13 +4790,13 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B112" s="2">
         <v>270171</v>
       </c>
       <c r="C112" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D112" t="s">
         <v>12</v>
@@ -4822,13 +4822,13 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B113" s="2">
         <v>270171</v>
       </c>
       <c r="C113" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D113" t="s">
         <v>12</v>
@@ -4854,13 +4854,13 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B114" s="2">
         <v>270171</v>
       </c>
       <c r="C114" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D114" t="s">
         <v>17</v>
@@ -4886,13 +4886,13 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B115" s="2">
         <v>270171</v>
       </c>
       <c r="C115" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D115" t="s">
         <v>17</v>
@@ -4918,13 +4918,13 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B116" s="2">
         <v>270171</v>
       </c>
       <c r="C116" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D116" t="s">
         <v>12</v>
@@ -4950,13 +4950,13 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B117" s="2">
         <v>270171</v>
       </c>
       <c r="C117" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D117" t="s">
         <v>12</v>
@@ -4982,13 +4982,13 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B118" s="2">
         <v>270171</v>
       </c>
       <c r="C118" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D118" t="s">
         <v>17</v>
@@ -5014,13 +5014,13 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B119" s="2">
         <v>270171</v>
       </c>
       <c r="C119" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D119" t="s">
         <v>12</v>
@@ -5046,13 +5046,13 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B120" s="2">
         <v>270171</v>
       </c>
       <c r="C120" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D120" t="s">
         <v>17</v>
@@ -5078,13 +5078,13 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B121" s="2">
         <v>270171</v>
       </c>
       <c r="C121" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D121" t="s">
         <v>17</v>
@@ -5110,13 +5110,13 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B122" s="2">
         <v>270170</v>
       </c>
       <c r="C122" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D122" t="s">
         <v>12</v>
@@ -5142,13 +5142,13 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B123" s="2">
         <v>270170</v>
       </c>
       <c r="C123" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D123" t="s">
         <v>12</v>
@@ -5174,13 +5174,13 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B124" s="2">
         <v>270170</v>
       </c>
       <c r="C124" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D124" t="s">
         <v>17</v>
@@ -5206,13 +5206,13 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B125" s="2">
         <v>270170</v>
       </c>
       <c r="C125" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D125" t="s">
         <v>17</v>
@@ -5238,13 +5238,13 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B126" s="2">
         <v>270170</v>
       </c>
       <c r="C126" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D126" t="s">
         <v>12</v>
@@ -5270,13 +5270,13 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B127" s="2">
         <v>270170</v>
       </c>
       <c r="C127" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D127" t="s">
         <v>12</v>
@@ -5302,13 +5302,13 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B128" s="2">
         <v>270170</v>
       </c>
       <c r="C128" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D128" t="s">
         <v>17</v>
@@ -5334,13 +5334,13 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B129" s="2">
         <v>270170</v>
       </c>
       <c r="C129" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D129" t="s">
         <v>12</v>
@@ -5366,13 +5366,13 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B130" s="2">
         <v>270170</v>
       </c>
       <c r="C130" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D130" t="s">
         <v>17</v>
@@ -5398,13 +5398,13 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B131" s="2">
         <v>270170</v>
       </c>
       <c r="C131" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D131" t="s">
         <v>17</v>
@@ -5430,7 +5430,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B132" s="2">
         <v>250900</v>
@@ -5462,7 +5462,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B133" s="2">
         <v>250900</v>
@@ -5494,7 +5494,7 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B134" s="2">
         <v>250900</v>
@@ -5526,7 +5526,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B135" s="2">
         <v>250900</v>
@@ -5558,7 +5558,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B136" s="2">
         <v>250900</v>
@@ -5590,7 +5590,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B137" s="2">
         <v>250900</v>
@@ -5622,13 +5622,13 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B138" s="2">
         <v>250470</v>
       </c>
       <c r="C138" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D138" t="s">
         <v>12</v>
@@ -5654,13 +5654,13 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B139" s="2">
         <v>250470</v>
       </c>
       <c r="C139" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D139" t="s">
         <v>12</v>
@@ -5686,13 +5686,13 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B140" s="2">
         <v>250470</v>
       </c>
       <c r="C140" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D140" t="s">
         <v>17</v>
@@ -5718,13 +5718,13 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B141" s="2">
         <v>250470</v>
       </c>
       <c r="C141" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D141" t="s">
         <v>17</v>
@@ -5750,7 +5750,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B142" s="2">
         <v>270440</v>
@@ -5782,7 +5782,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B143" s="2">
         <v>270440</v>
@@ -5814,7 +5814,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B144" s="2">
         <v>270440</v>
@@ -5846,7 +5846,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B145" s="2">
         <v>270440</v>
@@ -5878,7 +5878,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B146" s="2">
         <v>270440</v>
@@ -5910,7 +5910,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B147" s="2">
         <v>270440</v>
@@ -5942,7 +5942,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B148" s="2">
         <v>270440</v>
@@ -5974,7 +5974,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B149" s="2">
         <v>270440</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B150" s="2">
         <v>280645</v>
@@ -6038,7 +6038,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B151" s="2">
         <v>280645</v>
@@ -6070,7 +6070,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B152" s="2">
         <v>280645</v>
@@ -6102,7 +6102,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B153" s="2">
         <v>280645</v>
@@ -6134,7 +6134,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B154" s="2">
         <v>280645</v>
@@ -6166,7 +6166,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B155" s="2">
         <v>280645</v>
@@ -6198,13 +6198,13 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B156" s="2">
         <v>270900</v>
       </c>
       <c r="C156" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D156" t="s">
         <v>12</v>
@@ -6230,13 +6230,13 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B157" s="2">
         <v>270900</v>
       </c>
       <c r="C157" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D157" t="s">
         <v>12</v>
@@ -6262,13 +6262,13 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B158" s="2">
         <v>270900</v>
       </c>
       <c r="C158" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D158" t="s">
         <v>17</v>
@@ -6294,13 +6294,13 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B159" s="2">
         <v>270900</v>
       </c>
       <c r="C159" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D159" t="s">
         <v>17</v>
@@ -6326,13 +6326,13 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B160" s="2">
         <v>270900</v>
       </c>
       <c r="C160" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D160" t="s">
         <v>12</v>
@@ -6358,13 +6358,13 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B161" s="2">
         <v>270900</v>
       </c>
       <c r="C161" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D161" t="s">
         <v>12</v>
@@ -6390,7 +6390,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B162" s="2">
         <v>250050</v>
@@ -6422,7 +6422,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B163" s="2">
         <v>250050</v>
@@ -6454,7 +6454,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B164" s="2">
         <v>250050</v>
@@ -6486,7 +6486,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B165" s="2">
         <v>250050</v>
@@ -6518,7 +6518,7 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B166" s="2">
         <v>250050</v>
@@ -6550,7 +6550,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B167" s="2">
         <v>250050</v>
@@ -6582,7 +6582,7 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B168" s="2">
         <v>250050</v>
@@ -6614,7 +6614,7 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B169" s="2">
         <v>250050</v>
@@ -6646,7 +6646,7 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B170" s="2">
         <v>270410</v>
@@ -6678,7 +6678,7 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B171" s="2">
         <v>270410</v>
@@ -6710,13 +6710,13 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B172" s="2">
         <v>250512</v>
       </c>
       <c r="C172" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D172" t="s">
         <v>12</v>
@@ -6742,13 +6742,13 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B173" s="2">
         <v>250512</v>
       </c>
       <c r="C173" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D173" t="s">
         <v>12</v>
@@ -6774,13 +6774,13 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B174" s="2">
         <v>250512</v>
       </c>
       <c r="C174" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D174" t="s">
         <v>17</v>
@@ -6806,13 +6806,13 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B175" s="2">
         <v>250512</v>
       </c>
       <c r="C175" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D175" t="s">
         <v>17</v>
@@ -6838,7 +6838,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B176" s="2">
         <v>220050</v>
@@ -6870,7 +6870,7 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B177" s="2">
         <v>220050</v>
@@ -6902,7 +6902,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B178" s="2">
         <v>220050</v>
@@ -6934,7 +6934,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B179" s="2">
         <v>220050</v>
@@ -6966,7 +6966,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B180" s="2">
         <v>220050</v>
@@ -6998,7 +6998,7 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B181" s="2">
         <v>220050</v>
@@ -7030,7 +7030,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B182" s="2">
         <v>270293</v>
@@ -7062,7 +7062,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B183" s="2">
         <v>270293</v>
@@ -7094,7 +7094,7 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B184" s="2">
         <v>270293</v>
@@ -7126,7 +7126,7 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B185" s="2">
         <v>270293</v>
@@ -7158,7 +7158,7 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B186" s="2">
         <v>270293</v>
@@ -7190,7 +7190,7 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B187" s="2">
         <v>270293</v>
@@ -7222,7 +7222,7 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B188" s="2">
         <v>270293</v>
@@ -7254,7 +7254,7 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B189" s="2">
         <v>270293</v>
@@ -7286,7 +7286,7 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B190" s="2">
         <v>270460</v>
@@ -7318,7 +7318,7 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B191" s="2">
         <v>270460</v>
@@ -7350,7 +7350,7 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B192" s="2">
         <v>270460</v>
@@ -7382,7 +7382,7 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B193" s="2">
         <v>270460</v>
@@ -7414,7 +7414,7 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B194" s="2">
         <v>270460</v>
@@ -7446,7 +7446,7 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B195" s="2">
         <v>270460</v>
@@ -7478,7 +7478,7 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B196" s="2">
         <v>270460</v>
@@ -7510,7 +7510,7 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B197" s="2">
         <v>270460</v>
@@ -7542,13 +7542,13 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B198" s="2">
         <v>270380</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D198" t="s">
         <v>17</v>
@@ -7574,13 +7574,13 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B199" s="2">
         <v>270380</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D199" t="s">
         <v>12</v>
@@ -7606,13 +7606,13 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B200" s="2">
         <v>270380</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D200" t="s">
         <v>17</v>
@@ -7638,13 +7638,13 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B201" s="2">
         <v>270380</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D201" t="s">
         <v>17</v>
@@ -7670,13 +7670,13 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B202" s="2">
         <v>270380</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D202" t="s">
         <v>17</v>
@@ -7702,13 +7702,13 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B203" s="2">
         <v>270380</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D203" t="s">
         <v>12</v>
@@ -7734,13 +7734,13 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B204" s="2">
         <v>270380</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D204" t="s">
         <v>12</v>
@@ -7766,13 +7766,13 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B205" s="2">
         <v>270380</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D205" t="s">
         <v>12</v>
@@ -7798,13 +7798,13 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B206" s="2">
         <v>270380</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D206" t="s">
         <v>17</v>
@@ -7830,13 +7830,13 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B207" s="2">
         <v>270380</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D207" t="s">
         <v>12</v>
@@ -7862,7 +7862,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B208" s="2">
         <v>240150</v>
@@ -7894,7 +7894,7 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B209" s="2">
         <v>240150</v>
@@ -7926,7 +7926,7 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B210" s="2">
         <v>240150</v>
@@ -7958,7 +7958,7 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B211" s="2">
         <v>240150</v>
@@ -7990,7 +7990,7 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B212" s="2">
         <v>240150</v>
@@ -8022,7 +8022,7 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B213" s="2">
         <v>240150</v>
@@ -8054,13 +8054,13 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B214" s="2">
         <v>250510</v>
       </c>
       <c r="C214" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D214" t="s">
         <v>12</v>
@@ -8086,13 +8086,13 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B215" s="2">
         <v>250510</v>
       </c>
       <c r="C215" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D215" t="s">
         <v>12</v>
@@ -8118,13 +8118,13 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B216" s="2">
         <v>250510</v>
       </c>
       <c r="C216" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D216" t="s">
         <v>17</v>
@@ -8150,13 +8150,13 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B217" s="2">
         <v>250510</v>
       </c>
       <c r="C217" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D217" t="s">
         <v>17</v>
@@ -8662,7 +8662,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -8688,7 +8688,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -8714,7 +8714,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -8740,7 +8740,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8766,7 +8766,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -8792,7 +8792,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -8869,7 +8869,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -8895,7 +8895,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -8921,7 +8921,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -8947,7 +8947,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8973,7 +8973,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -8999,7 +8999,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -9081,7 +9081,7 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -9107,7 +9107,7 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -9133,7 +9133,7 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -9159,7 +9159,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -9185,7 +9185,7 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -9211,7 +9211,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -10136,14 +10136,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -10294,7 +10294,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -10320,7 +10320,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -10346,7 +10346,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -10372,7 +10372,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -10398,7 +10398,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -10424,7 +10424,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -10450,7 +10450,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -10476,7 +10476,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -10502,7 +10502,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -10528,7 +10528,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -10811,7 +10811,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -10837,7 +10837,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -10863,7 +10863,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -10889,7 +10889,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -10915,7 +10915,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -10941,7 +10941,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -10967,7 +10967,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -10993,7 +10993,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -11019,7 +11019,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -11045,7 +11045,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -11125,7 +11125,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -11151,7 +11151,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -11177,7 +11177,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -11203,7 +11203,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -11229,7 +11229,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -11255,7 +11255,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -11281,7 +11281,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -11307,7 +11307,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -11333,7 +11333,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -11359,7 +11359,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -11646,7 +11646,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -11672,7 +11672,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -11698,7 +11698,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -11724,7 +11724,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -12746,7 +12746,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -12772,7 +12772,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -12798,7 +12798,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -12824,7 +12824,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -12850,7 +12850,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -12876,7 +12876,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -13317,7 +13317,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -13343,7 +13343,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -13369,7 +13369,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -13395,7 +13395,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -14220,13 +14220,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="2">
         <v>270380</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -14252,13 +14252,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="2">
         <v>270380</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -14284,13 +14284,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="2">
         <v>270380</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -14316,13 +14316,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="2">
         <v>270380</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -14348,13 +14348,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2">
         <v>270380</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -14380,13 +14380,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="2">
         <v>270380</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -14412,13 +14412,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="2">
         <v>270380</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -14444,13 +14444,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" s="2">
         <v>270380</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -14476,13 +14476,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2">
         <v>270380</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -14508,13 +14508,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="2">
         <v>270380</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>

</xml_diff>